<commit_message>
update slyc model with the new version of the article
changed the network (sbml file) after SBC analysis and mass balance
changed the scripts (fba and extensions) to make them simpler
added mutant analysis for different scenarios
simplified the input folder
changed the output files generated by the scripts
updated readme files accordingly
</commit_message>
<xml_diff>
--- a/output/FBA_nitrogen_reduction.xlsx
+++ b/output/FBA_nitrogen_reduction.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="results_nitrogen_reduction" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B351"/>
+  <dimension ref="A1:B352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -383,7 +383,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.24</v>
+        <v>0.2399999999998793</v>
       </c>
     </row>
     <row r="3">
@@ -391,7 +391,7 @@
         <v>1.02</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2352941176469976</v>
+        <v>0.2352941176468451</v>
       </c>
     </row>
     <row r="4">
@@ -399,7 +399,7 @@
         <v>1.04</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2307692307692746</v>
+        <v>0.2307692307691072</v>
       </c>
     </row>
     <row r="5">
@@ -407,7 +407,7 @@
         <v>1.06</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2264150943398026</v>
+        <v>0.2264150943395408</v>
       </c>
     </row>
     <row r="6">
@@ -415,7 +415,7 @@
         <v>1.08</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2222222222222104</v>
+        <v>0.2222222222221287</v>
       </c>
     </row>
     <row r="7">
@@ -423,7 +423,7 @@
         <v>1.1</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2181818181818277</v>
+        <v>0.2181818181817319</v>
       </c>
     </row>
     <row r="8">
@@ -431,7 +431,7 @@
         <v>1.12</v>
       </c>
       <c r="B8" t="n">
-        <v>0.21428571428562</v>
+        <v>0.2142857142856757</v>
       </c>
     </row>
     <row r="9">
@@ -439,7 +439,7 @@
         <v>1.14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2105263157894424</v>
+        <v>0.2105263157893964</v>
       </c>
     </row>
     <row r="10">
@@ -447,7 +447,7 @@
         <v>1.16</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2068965517241092</v>
+        <v>0.2068965517248236</v>
       </c>
     </row>
     <row r="11">
@@ -455,7 +455,7 @@
         <v>1.18</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2033898305083795</v>
+        <v>0.203389830508374</v>
       </c>
     </row>
     <row r="12">
@@ -463,7 +463,7 @@
         <v>1.2</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2000000000001198</v>
+        <v>0.1999999999999371</v>
       </c>
     </row>
     <row r="13">
@@ -471,7 +471,7 @@
         <v>1.22</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1967213114752911</v>
+        <v>0.1967213114753308</v>
       </c>
     </row>
     <row r="14">
@@ -479,7 +479,7 @@
         <v>1.24</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1935483870966527</v>
+        <v>0.1935483870966927</v>
       </c>
     </row>
     <row r="15">
@@ -487,7 +487,7 @@
         <v>1.26</v>
       </c>
       <c r="B15" t="n">
-        <v>0.190476190476265</v>
+        <v>0.190476190476115</v>
       </c>
     </row>
     <row r="16">
@@ -495,7 +495,7 @@
         <v>1.28</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1874999999999215</v>
+        <v>0.1874999999999116</v>
       </c>
     </row>
     <row r="17">
@@ -503,7 +503,7 @@
         <v>1.3</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1846153846153331</v>
+        <v>0.1846153846153308</v>
       </c>
     </row>
     <row r="18">
@@ -511,7 +511,7 @@
         <v>1.32</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1818181818181299</v>
+        <v>0.1818181818181782</v>
       </c>
     </row>
     <row r="19">
@@ -519,7 +519,7 @@
         <v>1.34</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1791044776119388</v>
+        <v>0.1791044776119597</v>
       </c>
     </row>
     <row r="20">
@@ -527,7 +527,7 @@
         <v>1.36</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1764705882353689</v>
+        <v>0.1764705882353146</v>
       </c>
     </row>
     <row r="21">
@@ -535,7 +535,7 @@
         <v>1.38</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1739130434783036</v>
+        <v>0.1739130434781736</v>
       </c>
     </row>
     <row r="22">
@@ -543,7 +543,7 @@
         <v>1.4</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1714285714284847</v>
+        <v>0.1714285714281273</v>
       </c>
     </row>
     <row r="23">
@@ -551,7 +551,7 @@
         <v>1.42</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1690140845070846</v>
+        <v>0.1690140845069477</v>
       </c>
     </row>
     <row r="24">
@@ -559,7 +559,7 @@
         <v>1.44</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1666666666664963</v>
+        <v>0.1666666666665641</v>
       </c>
     </row>
     <row r="25">
@@ -567,7 +567,7 @@
         <v>1.46</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1643835616437796</v>
+        <v>0.1643835616438162</v>
       </c>
     </row>
     <row r="26">
@@ -575,7 +575,7 @@
         <v>1.48</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1621621621621199</v>
+        <v>0.1621621621620876</v>
       </c>
     </row>
     <row r="27">
@@ -583,7 +583,7 @@
         <v>1.5</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1600000000000006</v>
+        <v>0.1599999999999241</v>
       </c>
     </row>
     <row r="28">
@@ -591,7 +591,7 @@
         <v>1.52</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1578947368421347</v>
+        <v>0.1578947368420303</v>
       </c>
     </row>
     <row r="29">
@@ -599,7 +599,7 @@
         <v>1.54</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1558441558442281</v>
+        <v>0.1558441558440844</v>
       </c>
     </row>
     <row r="30">
@@ -607,7 +607,7 @@
         <v>1.56</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1538461538461802</v>
+        <v>0.1538461538460828</v>
       </c>
     </row>
     <row r="31">
@@ -615,7 +615,7 @@
         <v>1.580000000000001</v>
       </c>
       <c r="B31" t="n">
-        <v>0.151898734177151</v>
+        <v>0.151898734177146</v>
       </c>
     </row>
     <row r="32">
@@ -623,7 +623,7 @@
         <v>1.600000000000001</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1499999999999484</v>
+        <v>0.1499999999999389</v>
       </c>
     </row>
     <row r="33">
@@ -631,7 +631,7 @@
         <v>1.620000000000001</v>
       </c>
       <c r="B33" t="n">
-        <v>0.1481481481481453</v>
+        <v>0.1481481481480899</v>
       </c>
     </row>
     <row r="34">
@@ -639,7 +639,7 @@
         <v>1.640000000000001</v>
       </c>
       <c r="B34" t="n">
-        <v>0.146341463414572</v>
+        <v>0.1463414634145243</v>
       </c>
     </row>
     <row r="35">
@@ -647,7 +647,7 @@
         <v>1.660000000000001</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1445783132530053</v>
+        <v>0.14457831325287</v>
       </c>
     </row>
     <row r="36">
@@ -655,7 +655,7 @@
         <v>1.680000000000001</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1428571428571226</v>
+        <v>0.1428571428570759</v>
       </c>
     </row>
     <row r="37">
@@ -663,7 +663,7 @@
         <v>1.700000000000001</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1411764705882139</v>
+        <v>0.1411764705881662</v>
       </c>
     </row>
     <row r="38">
@@ -671,7 +671,7 @@
         <v>1.720000000000001</v>
       </c>
       <c r="B38" t="n">
-        <v>0.1395348837209011</v>
+        <v>0.1395348837208688</v>
       </c>
     </row>
     <row r="39">
@@ -679,7 +679,7 @@
         <v>1.740000000000001</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1379310344827384</v>
+        <v>0.1379310344826976</v>
       </c>
     </row>
     <row r="40">
@@ -687,7 +687,7 @@
         <v>1.760000000000001</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1363636363636119</v>
+        <v>0.1363636363635834</v>
       </c>
     </row>
     <row r="41">
@@ -695,7 +695,7 @@
         <v>1.780000000000001</v>
       </c>
       <c r="B41" t="n">
-        <v>0.1348314606741449</v>
+        <v>0.1348314606740988</v>
       </c>
     </row>
     <row r="42">
@@ -703,7 +703,7 @@
         <v>1.800000000000001</v>
       </c>
       <c r="B42" t="n">
-        <v>0.133333333333343</v>
+        <v>0.133333333333275</v>
       </c>
     </row>
     <row r="43">
@@ -711,7 +711,7 @@
         <v>1.820000000000001</v>
       </c>
       <c r="B43" t="n">
-        <v>0.1318681318680742</v>
+        <v>0.1318681318680806</v>
       </c>
     </row>
     <row r="44">
@@ -719,7 +719,7 @@
         <v>1.840000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.130434782608659</v>
+        <v>0.1304347826086433</v>
       </c>
     </row>
     <row r="45">
@@ -727,7 +727,7 @@
         <v>1.860000000000001</v>
       </c>
       <c r="B45" t="n">
-        <v>0.129032258064548</v>
+        <v>0.1290322580644532</v>
       </c>
     </row>
     <row r="46">
@@ -735,7 +735,7 @@
         <v>1.880000000000001</v>
       </c>
       <c r="B46" t="n">
-        <v>0.1276595744678941</v>
+        <v>0.1276595744680256</v>
       </c>
     </row>
     <row r="47">
@@ -743,7 +743,7 @@
         <v>1.900000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.1263157894736116</v>
+        <v>0.1263157894736433</v>
       </c>
     </row>
     <row r="48">
@@ -751,7 +751,7 @@
         <v>1.920000000000001</v>
       </c>
       <c r="B48" t="n">
-        <v>0.1249999999998326</v>
+        <v>0.1249999999999514</v>
       </c>
     </row>
     <row r="49">
@@ -759,7 +759,7 @@
         <v>1.940000000000001</v>
       </c>
       <c r="B49" t="n">
-        <v>0.1237113402062193</v>
+        <v>0.1237113402061724</v>
       </c>
     </row>
     <row r="50">
@@ -767,7 +767,7 @@
         <v>1.960000000000001</v>
       </c>
       <c r="B50" t="n">
-        <v>0.1224489795918424</v>
+        <v>0.1224489795918227</v>
       </c>
     </row>
     <row r="51">
@@ -775,7 +775,7 @@
         <v>1.980000000000001</v>
       </c>
       <c r="B51" t="n">
-        <v>0.1212121212121107</v>
+        <v>0.1212121212121064</v>
       </c>
     </row>
     <row r="52">
@@ -783,7 +783,7 @@
         <v>2.000000000000001</v>
       </c>
       <c r="B52" t="n">
-        <v>0.1199999999998819</v>
+        <v>0.1199999999998762</v>
       </c>
     </row>
     <row r="53">
@@ -791,7 +791,7 @@
         <v>2.020000000000001</v>
       </c>
       <c r="B53" t="n">
-        <v>0.1188118811879856</v>
+        <v>0.1188118811880571</v>
       </c>
     </row>
     <row r="54">
@@ -799,7 +799,7 @@
         <v>2.040000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.1176470588234622</v>
+        <v>0.1176470588234643</v>
       </c>
     </row>
     <row r="55">
@@ -807,7 +807,7 @@
         <v>2.060000000000001</v>
       </c>
       <c r="B55" t="n">
-        <v>0.1165048543688633</v>
+        <v>0.1165048543688881</v>
       </c>
     </row>
     <row r="56">
@@ -815,7 +815,7 @@
         <v>2.080000000000001</v>
       </c>
       <c r="B56" t="n">
-        <v>0.1153846153845654</v>
+        <v>0.1153846153845503</v>
       </c>
     </row>
     <row r="57">
@@ -823,7 +823,7 @@
         <v>2.100000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.1142857142856982</v>
+        <v>0.1142857142856836</v>
       </c>
     </row>
     <row r="58">
@@ -831,7 +831,7 @@
         <v>2.120000000000001</v>
       </c>
       <c r="B58" t="n">
-        <v>0.1132075471699042</v>
+        <v>0.1132075471697729</v>
       </c>
     </row>
     <row r="59">
@@ -839,7 +839,7 @@
         <v>2.140000000000001</v>
       </c>
       <c r="B59" t="n">
-        <v>0.1121495327100919</v>
+        <v>0.1121495327102043</v>
       </c>
     </row>
     <row r="60">
@@ -847,7 +847,7 @@
         <v>2.160000000000001</v>
       </c>
       <c r="B60" t="n">
-        <v>0.1111111111111114</v>
+        <v>0.1111111111110509</v>
       </c>
     </row>
     <row r="61">
@@ -855,7 +855,7 @@
         <v>2.180000000000001</v>
       </c>
       <c r="B61" t="n">
-        <v>0.1100917431191266</v>
+        <v>0.1100917431192073</v>
       </c>
     </row>
     <row r="62">
@@ -863,7 +863,7 @@
         <v>2.200000000000001</v>
       </c>
       <c r="B62" t="n">
-        <v>0.1090909090908799</v>
+        <v>0.1090909090908704</v>
       </c>
     </row>
     <row r="63">
@@ -871,7 +871,7 @@
         <v>2.220000000000001</v>
       </c>
       <c r="B63" t="n">
-        <v>0.1081081081080359</v>
+        <v>0.108108108108069</v>
       </c>
     </row>
     <row r="64">
@@ -879,7 +879,7 @@
         <v>2.240000000000001</v>
       </c>
       <c r="B64" t="n">
-        <v>0.1071428571428136</v>
+        <v>0.1071428571428253</v>
       </c>
     </row>
     <row r="65">
@@ -887,7 +887,7 @@
         <v>2.260000000000001</v>
       </c>
       <c r="B65" t="n">
-        <v>0.1061946902654476</v>
+        <v>0.1061946902654275</v>
       </c>
     </row>
     <row r="66">
@@ -895,7 +895,7 @@
         <v>2.280000000000001</v>
       </c>
       <c r="B66" t="n">
-        <v>0.1052631578948923</v>
+        <v>0.1052631578946952</v>
       </c>
     </row>
     <row r="67">
@@ -903,7 +903,7 @@
         <v>2.300000000000001</v>
       </c>
       <c r="B67" t="n">
-        <v>0.1043478260869093</v>
+        <v>0.104347826086913</v>
       </c>
     </row>
     <row r="68">
@@ -911,7 +911,7 @@
         <v>2.320000000000001</v>
       </c>
       <c r="B68" t="n">
-        <v>0.1034482758619528</v>
+        <v>0.1034482758620272</v>
       </c>
     </row>
     <row r="69">
@@ -919,7 +919,7 @@
         <v>2.340000000000001</v>
       </c>
       <c r="B69" t="n">
-        <v>0.1025641025640477</v>
+        <v>0.1025641025640556</v>
       </c>
     </row>
     <row r="70">
@@ -927,7 +927,7 @@
         <v>2.360000000000001</v>
       </c>
       <c r="B70" t="n">
-        <v>0.1016949152541903</v>
+        <v>0.1016949152541962</v>
       </c>
     </row>
     <row r="71">
@@ -935,7 +935,7 @@
         <v>2.380000000000001</v>
       </c>
       <c r="B71" t="n">
-        <v>0.1008403361343817</v>
+        <v>0.10084033613442</v>
       </c>
     </row>
     <row r="72">
@@ -943,7 +943,7 @@
         <v>2.400000000000001</v>
       </c>
       <c r="B72" t="n">
-        <v>0.09999999999991666</v>
+        <v>0.09999999999996147</v>
       </c>
     </row>
     <row r="73">
@@ -951,7 +951,7 @@
         <v>2.420000000000001</v>
       </c>
       <c r="B73" t="n">
-        <v>0.09917355371892142</v>
+        <v>0.09917355371897983</v>
       </c>
     </row>
     <row r="74">
@@ -959,7 +959,7 @@
         <v>2.440000000000001</v>
       </c>
       <c r="B74" t="n">
-        <v>0.09836065573754195</v>
+        <v>0.09836065573766474</v>
       </c>
     </row>
     <row r="75">
@@ -967,7 +967,7 @@
         <v>2.460000000000001</v>
       </c>
       <c r="B75" t="n">
-        <v>0.09756097560971652</v>
+        <v>0.09756097560971834</v>
       </c>
     </row>
     <row r="76">
@@ -975,7 +975,7 @@
         <v>2.480000000000001</v>
       </c>
       <c r="B76" t="n">
-        <v>0.09677419354832718</v>
+        <v>0.09677419354834321</v>
       </c>
     </row>
     <row r="77">
@@ -983,7 +983,7 @@
         <v>2.500000000000001</v>
       </c>
       <c r="B77" t="n">
-        <v>0.09599999999997881</v>
+        <v>0.09599999999997001</v>
       </c>
     </row>
     <row r="78">
@@ -991,7 +991,7 @@
         <v>2.520000000000001</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0952380952379954</v>
+        <v>0.09523809523804691</v>
       </c>
     </row>
     <row r="79">
@@ -999,7 +999,7 @@
         <v>2.540000000000001</v>
       </c>
       <c r="B79" t="n">
-        <v>0.09448818897626254</v>
+        <v>0.09448818897633014</v>
       </c>
     </row>
     <row r="80">
@@ -1007,7 +1007,7 @@
         <v>2.560000000000001</v>
       </c>
       <c r="B80" t="n">
-        <v>0.09375000000006529</v>
+        <v>0.09374999999995948</v>
       </c>
     </row>
     <row r="81">
@@ -1015,7 +1015,7 @@
         <v>2.580000000000001</v>
       </c>
       <c r="B81" t="n">
-        <v>0.09302325581397912</v>
+        <v>0.09302325581392241</v>
       </c>
     </row>
     <row r="82">
@@ -1023,7 +1023,7 @@
         <v>2.600000000000001</v>
       </c>
       <c r="B82" t="n">
-        <v>0.09230769230766908</v>
+        <v>0.09230769230788287</v>
       </c>
     </row>
     <row r="83">
@@ -1031,7 +1031,7 @@
         <v>2.620000000000001</v>
       </c>
       <c r="B83" t="n">
-        <v>0.09160305343513742</v>
+        <v>0.09160305343507059</v>
       </c>
     </row>
     <row r="84">
@@ -1039,7 +1039,7 @@
         <v>2.640000000000001</v>
       </c>
       <c r="B84" t="n">
-        <v>0.09090909090910194</v>
+        <v>0.09090909090905558</v>
       </c>
     </row>
     <row r="85">
@@ -1047,7 +1047,7 @@
         <v>2.660000000000001</v>
       </c>
       <c r="B85" t="n">
-        <v>0.09022556390975199</v>
+        <v>0.09022556390918582</v>
       </c>
     </row>
     <row r="86">
@@ -1055,7 +1055,7 @@
         <v>2.680000000000001</v>
       </c>
       <c r="B86" t="n">
-        <v>0.08955223880583182</v>
+        <v>0.08955223880538186</v>
       </c>
     </row>
     <row r="87">
@@ -1063,7 +1063,7 @@
         <v>2.700000000000002</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0888888888889432</v>
+        <v>0.08888888888886599</v>
       </c>
     </row>
     <row r="88">
@@ -1071,7 +1071,7 @@
         <v>2.720000000000002</v>
       </c>
       <c r="B88" t="n">
-        <v>0.08823529411758671</v>
+        <v>0.08823529411762618</v>
       </c>
     </row>
     <row r="89">
@@ -1079,7 +1079,7 @@
         <v>2.740000000000002</v>
       </c>
       <c r="B89" t="n">
-        <v>0.08759124087591419</v>
+        <v>0.08759124087589087</v>
       </c>
     </row>
     <row r="90">
@@ -1087,7 +1087,7 @@
         <v>2.760000000000002</v>
       </c>
       <c r="B90" t="n">
-        <v>0.08695652173922296</v>
+        <v>0.08695652173910808</v>
       </c>
     </row>
     <row r="91">
@@ -1095,7 +1095,7 @@
         <v>2.780000000000002</v>
       </c>
       <c r="B91" t="n">
-        <v>0.08633093525171308</v>
+        <v>0.08633093525178061</v>
       </c>
     </row>
     <row r="92">
@@ -1103,7 +1103,7 @@
         <v>2.800000000000002</v>
       </c>
       <c r="B92" t="n">
-        <v>0.08571428571413921</v>
+        <v>0.08571428571421258</v>
       </c>
     </row>
     <row r="93">
@@ -1111,7 +1111,7 @@
         <v>2.820000000000002</v>
       </c>
       <c r="B93" t="n">
-        <v>0.08510638297880443</v>
+        <v>0.08510638297863858</v>
       </c>
     </row>
     <row r="94">
@@ -1119,7 +1119,7 @@
         <v>2.840000000000002</v>
       </c>
       <c r="B94" t="n">
-        <v>0.08450704225357772</v>
+        <v>0.08450704225344019</v>
       </c>
     </row>
     <row r="95">
@@ -1127,7 +1127,7 @@
         <v>2.860000000000002</v>
       </c>
       <c r="B95" t="n">
-        <v>0.08391608391612494</v>
+        <v>0.08391608391600235</v>
       </c>
     </row>
     <row r="96">
@@ -1135,7 +1135,7 @@
         <v>2.880000000000002</v>
       </c>
       <c r="B96" t="n">
-        <v>0.08333333333324486</v>
+        <v>0.08333333333325108</v>
       </c>
     </row>
     <row r="97">
@@ -1143,7 +1143,7 @@
         <v>2.900000000000002</v>
       </c>
       <c r="B97" t="n">
-        <v>0.0827586206894306</v>
+        <v>0.0827586206896216</v>
       </c>
     </row>
     <row r="98">
@@ -1151,7 +1151,7 @@
         <v>2.920000000000002</v>
       </c>
       <c r="B98" t="n">
-        <v>0.08219178082193083</v>
+        <v>0.08219178082188298</v>
       </c>
     </row>
     <row r="99">
@@ -1159,7 +1159,7 @@
         <v>2.940000000000002</v>
       </c>
       <c r="B99" t="n">
-        <v>0.08163265306127256</v>
+        <v>0.08163265306117344</v>
       </c>
     </row>
     <row r="100">
@@ -1167,7 +1167,7 @@
         <v>2.960000000000002</v>
       </c>
       <c r="B100" t="n">
-        <v>0.08108108108099399</v>
+        <v>0.08108108108104618</v>
       </c>
     </row>
     <row r="101">
@@ -1175,7 +1175,7 @@
         <v>2.980000000000002</v>
       </c>
       <c r="B101" t="n">
-        <v>0.08053691275164192</v>
+        <v>0.08053691275164608</v>
       </c>
     </row>
     <row r="102">
@@ -1183,7 +1183,7 @@
         <v>3.000000000000002</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0799999999999656</v>
+        <v>0.08000000000002085</v>
       </c>
     </row>
     <row r="103">
@@ -1191,7 +1191,7 @@
         <v>3.020000000000002</v>
       </c>
       <c r="B103" t="n">
-        <v>0.07947019867546995</v>
+        <v>0.07947019867544154</v>
       </c>
     </row>
     <row r="104">
@@ -1199,7 +1199,7 @@
         <v>3.040000000000002</v>
       </c>
       <c r="B104" t="n">
-        <v>0.07894736842093136</v>
+        <v>0.07894736842099034</v>
       </c>
     </row>
     <row r="105">
@@ -1207,7 +1207,7 @@
         <v>3.060000000000002</v>
       </c>
       <c r="B105" t="n">
-        <v>0.07843137254904133</v>
+        <v>0.07843137254896562</v>
       </c>
     </row>
     <row r="106">
@@ -1215,7 +1215,7 @@
         <v>3.080000000000002</v>
       </c>
       <c r="B106" t="n">
-        <v>0.07792207792214728</v>
+        <v>0.0779220779220217</v>
       </c>
     </row>
     <row r="107">
@@ -1223,7 +1223,7 @@
         <v>3.100000000000002</v>
       </c>
       <c r="B107" t="n">
-        <v>0.07741935483868581</v>
+        <v>0.07741935483865037</v>
       </c>
     </row>
     <row r="108">
@@ -1231,7 +1231,7 @@
         <v>3.120000000000002</v>
       </c>
       <c r="B108" t="n">
-        <v>0.07692307692302498</v>
+        <v>0.07692307692302675</v>
       </c>
     </row>
     <row r="109">
@@ -1239,7 +1239,7 @@
         <v>3.140000000000002</v>
       </c>
       <c r="B109" t="n">
-        <v>0.07643312101911544</v>
+        <v>0.07643312101904642</v>
       </c>
     </row>
     <row r="110">
@@ -1247,7 +1247,7 @@
         <v>3.160000000000002</v>
       </c>
       <c r="B110" t="n">
-        <v>0.07594936708851067</v>
+        <v>0.07594936708853804</v>
       </c>
     </row>
     <row r="111">
@@ -1255,7 +1255,7 @@
         <v>3.180000000000002</v>
       </c>
       <c r="B111" t="n">
-        <v>0.07547169811304355</v>
+        <v>0.07547169811311609</v>
       </c>
     </row>
     <row r="112">
@@ -1263,7 +1263,7 @@
         <v>3.200000000000002</v>
       </c>
       <c r="B112" t="n">
-        <v>0.07500000000008042</v>
+        <v>0.07499999999989881</v>
       </c>
     </row>
     <row r="113">
@@ -1271,7 +1271,7 @@
         <v>3.220000000000002</v>
       </c>
       <c r="B113" t="n">
-        <v>0.07453416149074799</v>
+        <v>0.07453416149057604</v>
       </c>
     </row>
     <row r="114">
@@ -1279,7 +1279,7 @@
         <v>3.240000000000002</v>
       </c>
       <c r="B114" t="n">
-        <v>0.07407407407393843</v>
+        <v>0.07407407407404613</v>
       </c>
     </row>
     <row r="115">
@@ -1287,7 +1287,7 @@
         <v>3.260000000000002</v>
       </c>
       <c r="B115" t="n">
-        <v>0.07361963190182415</v>
+        <v>0.07361963190179237</v>
       </c>
     </row>
     <row r="116">
@@ -1295,7 +1295,7 @@
         <v>3.280000000000002</v>
       </c>
       <c r="B116" t="n">
-        <v>0.07317073170721573</v>
+        <v>0.07317073170726975</v>
       </c>
     </row>
     <row r="117">
@@ -1303,7 +1303,7 @@
         <v>3.300000000000002</v>
       </c>
       <c r="B117" t="n">
-        <v>0.07272727272711417</v>
+        <v>0.07272727272722444</v>
       </c>
     </row>
     <row r="118">
@@ -1311,7 +1311,7 @@
         <v>3.320000000000002</v>
       </c>
       <c r="B118" t="n">
-        <v>0.07228915662639546</v>
+        <v>0.07228915662645852</v>
       </c>
     </row>
     <row r="119">
@@ -1319,7 +1319,7 @@
         <v>3.340000000000002</v>
       </c>
       <c r="B119" t="n">
-        <v>0.07185628742497385</v>
+        <v>0.07185628742509935</v>
       </c>
     </row>
     <row r="120">
@@ -1327,7 +1327,7 @@
         <v>3.360000000000002</v>
       </c>
       <c r="B120" t="n">
-        <v>0.07142857142856002</v>
+        <v>0.07142857142858082</v>
       </c>
     </row>
     <row r="121">
@@ -1335,7 +1335,7 @@
         <v>3.380000000000002</v>
       </c>
       <c r="B121" t="n">
-        <v>0.07100591715971891</v>
+        <v>0.07100591715977123</v>
       </c>
     </row>
     <row r="122">
@@ -1343,7 +1343,7 @@
         <v>3.400000000000002</v>
       </c>
       <c r="B122" t="n">
-        <v>0.07058823529397207</v>
+        <v>0.07058823529400744</v>
       </c>
     </row>
     <row r="123">
@@ -1351,7 +1351,7 @@
         <v>3.420000000000002</v>
       </c>
       <c r="B123" t="n">
-        <v>0.07017543859643205</v>
+        <v>0.07017543859638982</v>
       </c>
     </row>
     <row r="124">
@@ -1359,7 +1359,7 @@
         <v>3.440000000000002</v>
       </c>
       <c r="B124" t="n">
-        <v>0.06976744186045204</v>
+        <v>0.06976744186042681</v>
       </c>
     </row>
     <row r="125">
@@ -1367,7 +1367,7 @@
         <v>3.460000000000002</v>
       </c>
       <c r="B125" t="n">
-        <v>0.06936416184981335</v>
+        <v>0.06936416184965381</v>
       </c>
     </row>
     <row r="126">
@@ -1375,7 +1375,7 @@
         <v>3.480000000000002</v>
       </c>
       <c r="B126" t="n">
-        <v>0.06896551724130161</v>
+        <v>0.06896551724136482</v>
       </c>
     </row>
     <row r="127">
@@ -1383,7 +1383,7 @@
         <v>3.500000000000002</v>
       </c>
       <c r="B127" t="n">
-        <v>0.06857142857141797</v>
+        <v>0.06857142857127291</v>
       </c>
     </row>
     <row r="128">
@@ -1391,7 +1391,7 @@
         <v>3.520000000000002</v>
       </c>
       <c r="B128" t="n">
-        <v>0.06818181818172141</v>
+        <v>0.06818181818178927</v>
       </c>
     </row>
     <row r="129">
@@ -1399,7 +1399,7 @@
         <v>3.540000000000002</v>
       </c>
       <c r="B129" t="n">
-        <v>0.06779661016952002</v>
+        <v>0.06779661016947922</v>
       </c>
     </row>
     <row r="130">
@@ -1407,7 +1407,7 @@
         <v>3.560000000000002</v>
       </c>
       <c r="B130" t="n">
-        <v>0.06741573033709272</v>
+        <v>0.06741573033704183</v>
       </c>
     </row>
     <row r="131">
@@ -1415,7 +1415,7 @@
         <v>3.580000000000002</v>
       </c>
       <c r="B131" t="n">
-        <v>0.06703910614507258</v>
+        <v>0.0670391061452114</v>
       </c>
     </row>
     <row r="132">
@@ -1423,7 +1423,7 @@
         <v>3.600000000000002</v>
       </c>
       <c r="B132" t="n">
-        <v>0.06666666666649831</v>
+        <v>0.0666666666665699</v>
       </c>
     </row>
     <row r="133">
@@ -1431,7 +1431,7 @@
         <v>3.620000000000002</v>
       </c>
       <c r="B133" t="n">
-        <v>0.0662983425414569</v>
+        <v>0.0662983425413697</v>
       </c>
     </row>
     <row r="134">
@@ -1439,7 +1439,7 @@
         <v>3.640000000000002</v>
       </c>
       <c r="B134" t="n">
-        <v>0.06593406593405347</v>
+        <v>0.0659340659340231</v>
       </c>
     </row>
     <row r="135">
@@ -1447,7 +1447,7 @@
         <v>3.660000000000002</v>
       </c>
       <c r="B135" t="n">
-        <v>0.06557377049174855</v>
+        <v>0.06557377049178503</v>
       </c>
     </row>
     <row r="136">
@@ -1455,7 +1455,7 @@
         <v>3.680000000000002</v>
       </c>
       <c r="B136" t="n">
-        <v>0.06521739130419901</v>
+        <v>0.06521739130433819</v>
       </c>
     </row>
     <row r="137">
@@ -1463,7 +1463,7 @@
         <v>3.700000000000002</v>
       </c>
       <c r="B137" t="n">
-        <v>0.06486486486492002</v>
+        <v>0.06486486486485152</v>
       </c>
     </row>
     <row r="138">
@@ -1471,7 +1471,7 @@
         <v>3.720000000000002</v>
       </c>
       <c r="B138" t="n">
-        <v>0.0645161290324331</v>
+        <v>0.06451612903221202</v>
       </c>
     </row>
     <row r="139">
@@ -1479,7 +1479,7 @@
         <v>3.740000000000002</v>
       </c>
       <c r="B139" t="n">
-        <v>0.06417112299450675</v>
+        <v>0.06417112299462119</v>
       </c>
     </row>
     <row r="140">
@@ -1487,7 +1487,7 @@
         <v>3.760000000000002</v>
       </c>
       <c r="B140" t="n">
-        <v>0.06382978723408117</v>
+        <v>0.06382978723401167</v>
       </c>
     </row>
     <row r="141">
@@ -1495,7 +1495,7 @@
         <v>3.780000000000002</v>
       </c>
       <c r="B141" t="n">
-        <v>0.06349206349211545</v>
+        <v>0.06349206349203398</v>
       </c>
     </row>
     <row r="142">
@@ -1503,7 +1503,7 @@
         <v>3.800000000000002</v>
       </c>
       <c r="B142" t="n">
-        <v>0.06315789473700224</v>
+        <v>0.06315789473681334</v>
       </c>
     </row>
     <row r="143">
@@ -1511,7 +1511,7 @@
         <v>3.820000000000003</v>
       </c>
       <c r="B143" t="n">
-        <v>0.06282722513090311</v>
+        <v>0.06282722513086014</v>
       </c>
     </row>
     <row r="144">
@@ -1519,7 +1519,7 @@
         <v>3.840000000000003</v>
       </c>
       <c r="B144" t="n">
-        <v>0.06249999999993692</v>
+        <v>0.06249999999997301</v>
       </c>
     </row>
     <row r="145">
@@ -1527,7 +1527,7 @@
         <v>3.860000000000003</v>
       </c>
       <c r="B145" t="n">
-        <v>0.06217616580319368</v>
+        <v>0.06217616580308955</v>
       </c>
     </row>
     <row r="146">
@@ -1535,7 +1535,7 @@
         <v>3.880000000000003</v>
       </c>
       <c r="B146" t="n">
-        <v>0.0618556701031218</v>
+        <v>0.06185567010304174</v>
       </c>
     </row>
     <row r="147">
@@ -1543,7 +1543,7 @@
         <v>3.900000000000003</v>
       </c>
       <c r="B147" t="n">
-        <v>0.06153846153846992</v>
+        <v>0.06153846153843217</v>
       </c>
     </row>
     <row r="148">
@@ -1551,7 +1551,7 @@
         <v>3.920000000000003</v>
       </c>
       <c r="B148" t="n">
-        <v>0.0612244897957623</v>
+        <v>0.06122448979591363</v>
       </c>
     </row>
     <row r="149">
@@ -1559,7 +1559,7 @@
         <v>3.940000000000003</v>
       </c>
       <c r="B149" t="n">
-        <v>0.06091370558392584</v>
+        <v>0.06091370558375378</v>
       </c>
     </row>
     <row r="150">
@@ -1567,7 +1567,7 @@
         <v>3.960000000000003</v>
       </c>
       <c r="B150" t="n">
-        <v>0.06060606060613027</v>
+        <v>0.06060606060605025</v>
       </c>
     </row>
     <row r="151">
@@ -1575,7 +1575,7 @@
         <v>3.980000000000003</v>
       </c>
       <c r="B151" t="n">
-        <v>0.06030150753771693</v>
+        <v>0.06030150753766932</v>
       </c>
     </row>
     <row r="152">
@@ -1583,7 +1583,7 @@
         <v>4.000000000000003</v>
       </c>
       <c r="B152" t="n">
-        <v>0.05999999999981622</v>
+        <v>0.05999999999996319</v>
       </c>
     </row>
     <row r="153">
@@ -1591,7 +1591,7 @@
         <v>4.020000000000003</v>
       </c>
       <c r="B153" t="n">
-        <v>0.05970149253750663</v>
+        <v>0.0597014925371333</v>
       </c>
     </row>
     <row r="154">
@@ -1599,7 +1599,7 @@
         <v>4.040000000000003</v>
       </c>
       <c r="B154" t="n">
-        <v>0.05940594059384573</v>
+        <v>0.05940594059397132</v>
       </c>
     </row>
     <row r="155">
@@ -1607,7 +1607,7 @@
         <v>4.060000000000002</v>
       </c>
       <c r="B155" t="n">
-        <v>0.059113300492526</v>
+        <v>0.05911330049254713</v>
       </c>
     </row>
     <row r="156">
@@ -1615,7 +1615,7 @@
         <v>4.080000000000003</v>
       </c>
       <c r="B156" t="n">
-        <v>0.05882352941156917</v>
+        <v>0.05882352941155728</v>
       </c>
     </row>
     <row r="157">
@@ -1623,7 +1623,7 @@
         <v>4.100000000000003</v>
       </c>
       <c r="B157" t="n">
-        <v>0.05853658536588712</v>
+        <v>0.05853658536571188</v>
       </c>
     </row>
     <row r="158">
@@ -1631,7 +1631,7 @@
         <v>4.120000000000003</v>
       </c>
       <c r="B158" t="n">
-        <v>0.05825242718448032</v>
+        <v>0.05825242718446028</v>
       </c>
     </row>
     <row r="159">
@@ -1639,7 +1639,7 @@
         <v>4.140000000000002</v>
       </c>
       <c r="B159" t="n">
-        <v>0.05797101449264775</v>
+        <v>0.057971014492668</v>
       </c>
     </row>
     <row r="160">
@@ -1647,7 +1647,7 @@
         <v>4.160000000000003</v>
       </c>
       <c r="B160" t="n">
-        <v>0.0576923076922855</v>
+        <v>0.05769230769222463</v>
       </c>
     </row>
     <row r="161">
@@ -1655,7 +1655,7 @@
         <v>4.180000000000003</v>
       </c>
       <c r="B161" t="n">
-        <v>0.05741626794255915</v>
+        <v>0.0574162679424875</v>
       </c>
     </row>
     <row r="162">
@@ -1663,7 +1663,7 @@
         <v>4.200000000000003</v>
       </c>
       <c r="B162" t="n">
-        <v>0.05714285714289349</v>
+        <v>0.05714285714281949</v>
       </c>
     </row>
     <row r="163">
@@ -1671,7 +1671,7 @@
         <v>4.220000000000002</v>
       </c>
       <c r="B163" t="n">
-        <v>0.05687203791473518</v>
+        <v>0.05687203791466722</v>
       </c>
     </row>
     <row r="164">
@@ -1679,7 +1679,7 @@
         <v>4.240000000000003</v>
       </c>
       <c r="B164" t="n">
-        <v>0.05660377358481808</v>
+        <v>0.05660377358488836</v>
       </c>
     </row>
     <row r="165">
@@ -1687,7 +1687,7 @@
         <v>4.260000000000003</v>
       </c>
       <c r="B165" t="n">
-        <v>0.05633802816906508</v>
+        <v>0.05633802816900196</v>
       </c>
     </row>
     <row r="166">
@@ -1695,7 +1695,7 @@
         <v>4.280000000000003</v>
       </c>
       <c r="B166" t="n">
-        <v>0.05607476635526921</v>
+        <v>0.05607476635512218</v>
       </c>
     </row>
     <row r="167">
@@ -1703,7 +1703,7 @@
         <v>4.300000000000002</v>
       </c>
       <c r="B167" t="n">
-        <v>0.05581395348839607</v>
+        <v>0.05581395348832385</v>
       </c>
     </row>
     <row r="168">
@@ -1711,7 +1711,7 @@
         <v>4.320000000000003</v>
       </c>
       <c r="B168" t="n">
-        <v>0.05555555555539064</v>
+        <v>0.05555555555550563</v>
       </c>
     </row>
     <row r="169">
@@ -1719,7 +1719,7 @@
         <v>4.340000000000003</v>
       </c>
       <c r="B169" t="n">
-        <v>0.05529953917055756</v>
+        <v>0.05529953917057429</v>
       </c>
     </row>
     <row r="170">
@@ -1727,7 +1727,7 @@
         <v>4.360000000000003</v>
       </c>
       <c r="B170" t="n">
-        <v>0.05504587155981059</v>
+        <v>0.05504587155967736</v>
       </c>
     </row>
     <row r="171">
@@ -1735,7 +1735,7 @@
         <v>4.380000000000003</v>
       </c>
       <c r="B171" t="n">
-        <v>0.05479452054794334</v>
+        <v>0.05479452054807458</v>
       </c>
     </row>
     <row r="172">
@@ -1743,7 +1743,7 @@
         <v>4.400000000000003</v>
       </c>
       <c r="B172" t="n">
-        <v>0.05454545454524085</v>
+        <v>0.05454545454557059</v>
       </c>
     </row>
     <row r="173">
@@ -1751,7 +1751,7 @@
         <v>4.420000000000003</v>
       </c>
       <c r="B173" t="n">
-        <v>0.05429864253394621</v>
+        <v>0.05429864253405987</v>
       </c>
     </row>
     <row r="174">
@@ -1759,7 +1759,7 @@
         <v>4.440000000000003</v>
       </c>
       <c r="B174" t="n">
-        <v>0.05405405405410341</v>
+        <v>0.05405405405403226</v>
       </c>
     </row>
     <row r="175">
@@ -1767,7 +1767,7 @@
         <v>4.460000000000003</v>
       </c>
       <c r="B175" t="n">
-        <v>0.05381165919273939</v>
+        <v>0.05381165919281963</v>
       </c>
     </row>
     <row r="176">
@@ -1775,7 +1775,7 @@
         <v>4.480000000000003</v>
       </c>
       <c r="B176" t="n">
-        <v>0.05357142857148964</v>
+        <v>0.05357142857142582</v>
       </c>
     </row>
     <row r="177">
@@ -1783,7 +1783,7 @@
         <v>4.500000000000004</v>
       </c>
       <c r="B177" t="n">
-        <v>0.05333333333345951</v>
+        <v>0.05333333333332487</v>
       </c>
     </row>
     <row r="178">
@@ -1791,7 +1791,7 @@
         <v>4.520000000000003</v>
       </c>
       <c r="B178" t="n">
-        <v>0.0530973451327461</v>
+        <v>0.05309734513268482</v>
       </c>
     </row>
     <row r="179">
@@ -1799,7 +1799,7 @@
         <v>4.540000000000003</v>
       </c>
       <c r="B179" t="n">
-        <v>0.05286343612339518</v>
+        <v>0.05286343612334504</v>
       </c>
     </row>
     <row r="180">
@@ -1807,7 +1807,7 @@
         <v>4.560000000000003</v>
       </c>
       <c r="B180" t="n">
-        <v>0.05263157894734118</v>
+        <v>0.05263157894733952</v>
       </c>
     </row>
     <row r="181">
@@ -1815,7 +1815,7 @@
         <v>4.580000000000004</v>
       </c>
       <c r="B181" t="n">
-        <v>0.0524017467250884</v>
+        <v>0.05240174672486503</v>
       </c>
     </row>
     <row r="182">
@@ -1823,7 +1823,7 @@
         <v>4.600000000000003</v>
       </c>
       <c r="B182" t="n">
-        <v>0.05217391304340514</v>
+        <v>0.05217391304345808</v>
       </c>
     </row>
     <row r="183">
@@ -1831,7 +1831,7 @@
         <v>4.620000000000003</v>
       </c>
       <c r="B183" t="n">
-        <v>0.05194805194801739</v>
+        <v>0.05194805194803195</v>
       </c>
     </row>
     <row r="184">
@@ -1839,7 +1839,7 @@
         <v>4.640000000000003</v>
       </c>
       <c r="B184" t="n">
-        <v>0.05172413793107076</v>
+        <v>0.05172413793101403</v>
       </c>
     </row>
     <row r="185">
@@ -1847,7 +1847,7 @@
         <v>4.660000000000004</v>
       </c>
       <c r="B185" t="n">
-        <v>0.05150214592258515</v>
+        <v>0.05150214592269402</v>
       </c>
     </row>
     <row r="186">
@@ -1855,7 +1855,7 @@
         <v>4.680000000000003</v>
       </c>
       <c r="B186" t="n">
-        <v>0.05128205128190115</v>
+        <v>0.0512820512820579</v>
       </c>
     </row>
     <row r="187">
@@ -1863,7 +1863,7 @@
         <v>4.700000000000003</v>
       </c>
       <c r="B187" t="n">
-        <v>0.05106382978708607</v>
+        <v>0.05106382978721244</v>
       </c>
     </row>
     <row r="188">
@@ -1871,7 +1871,7 @@
         <v>4.720000000000003</v>
       </c>
       <c r="B188" t="n">
-        <v>0.05084745762709511</v>
+        <v>0.05084745762709638</v>
       </c>
     </row>
     <row r="189">
@@ -1879,7 +1879,7 @@
         <v>4.740000000000004</v>
       </c>
       <c r="B189" t="n">
-        <v>0.05063291139241913</v>
+        <v>0.0506329113923844</v>
       </c>
     </row>
     <row r="190">
@@ -1887,7 +1887,7 @@
         <v>4.760000000000003</v>
       </c>
       <c r="B190" t="n">
-        <v>0.0504201680671137</v>
+        <v>0.05042016806720451</v>
       </c>
     </row>
     <row r="191">
@@ -1895,7 +1895,7 @@
         <v>4.780000000000003</v>
       </c>
       <c r="B191" t="n">
-        <v>0.05020920502079377</v>
+        <v>0.05020920502089726</v>
       </c>
     </row>
     <row r="192">
@@ -1903,7 +1903,7 @@
         <v>4.800000000000003</v>
       </c>
       <c r="B192" t="n">
-        <v>0.04999999999998198</v>
+        <v>0.04999999999997787</v>
       </c>
     </row>
     <row r="193">
@@ -1911,7 +1911,7 @@
         <v>4.820000000000004</v>
       </c>
       <c r="B193" t="n">
-        <v>0.04979253112031934</v>
+        <v>0.04979253112031211</v>
       </c>
     </row>
     <row r="194">
@@ -1919,7 +1919,7 @@
         <v>4.840000000000003</v>
       </c>
       <c r="B194" t="n">
-        <v>0.0495867768596273</v>
+        <v>0.04958677685948409</v>
       </c>
     </row>
     <row r="195">
@@ -1927,7 +1927,7 @@
         <v>4.860000000000003</v>
       </c>
       <c r="B195" t="n">
-        <v>0.04938271604926571</v>
+        <v>0.04938271604936255</v>
       </c>
     </row>
     <row r="196">
@@ -1935,7 +1935,7 @@
         <v>4.880000000000003</v>
       </c>
       <c r="B196" t="n">
-        <v>0.04918032786900293</v>
+        <v>0.04918032786881216</v>
       </c>
     </row>
     <row r="197">
@@ -1943,7 +1943,7 @@
         <v>4.900000000000004</v>
       </c>
       <c r="B197" t="n">
-        <v>0.0489795918365811</v>
+        <v>0.04897959183671414</v>
       </c>
     </row>
     <row r="198">
@@ -1951,7 +1951,7 @@
         <v>4.920000000000003</v>
       </c>
       <c r="B198" t="n">
-        <v>0.0487804878048272</v>
+        <v>0.04878048780486084</v>
       </c>
     </row>
     <row r="199">
@@ -1959,7 +1959,7 @@
         <v>4.940000000000003</v>
       </c>
       <c r="B199" t="n">
-        <v>0.04858299595138363</v>
+        <v>0.04858299595137107</v>
       </c>
     </row>
     <row r="200">
@@ -1967,7 +1967,7 @@
         <v>4.960000000000004</v>
       </c>
       <c r="B200" t="n">
-        <v>0.04838709677414515</v>
+        <v>0.04838709677414795</v>
       </c>
     </row>
     <row r="201">
@@ -1975,7 +1975,7 @@
         <v>4.980000000000004</v>
       </c>
       <c r="B201" t="n">
-        <v>0.04819277108438203</v>
+        <v>0.04819277108428957</v>
       </c>
     </row>
     <row r="202">
@@ -1983,7 +1983,7 @@
         <v>5.000000000000004</v>
       </c>
       <c r="B202" t="n">
-        <v>0.04799999999981381</v>
+        <v>0.04799999999995323</v>
       </c>
     </row>
     <row r="203">
@@ -1991,7 +1991,7 @@
         <v>5.020000000000003</v>
       </c>
       <c r="B203" t="n">
-        <v>0.04780876494021088</v>
+        <v>0.04780876494019344</v>
       </c>
     </row>
     <row r="204">
@@ -1999,7 +1999,7 @@
         <v>5.040000000000004</v>
       </c>
       <c r="B204" t="n">
-        <v>0.04761904761885954</v>
+        <v>0.0476190476190033</v>
       </c>
     </row>
     <row r="205">
@@ -2007,7 +2007,7 @@
         <v>5.060000000000004</v>
       </c>
       <c r="B205" t="n">
-        <v>0.04743083003941799</v>
+        <v>0.04743083003950699</v>
       </c>
     </row>
     <row r="206">
@@ -2015,7 +2015,7 @@
         <v>5.080000000000004</v>
       </c>
       <c r="B206" t="n">
-        <v>0.04724409448818846</v>
+        <v>0.04724409448817074</v>
       </c>
     </row>
     <row r="207">
@@ -2023,7 +2023,7 @@
         <v>5.100000000000003</v>
       </c>
       <c r="B207" t="n">
-        <v>0.04705882352912685</v>
+        <v>0.04705882352939355</v>
       </c>
     </row>
     <row r="208">
@@ -2031,7 +2031,7 @@
         <v>5.120000000000004</v>
       </c>
       <c r="B208" t="n">
-        <v>0.04687499999977305</v>
+        <v>0.04687499999998131</v>
       </c>
     </row>
     <row r="209">
@@ -2039,7 +2039,7 @@
         <v>5.140000000000004</v>
       </c>
       <c r="B209" t="n">
-        <v>0.04669260700373642</v>
+        <v>0.04669260700387401</v>
       </c>
     </row>
     <row r="210">
@@ -2047,7 +2047,7 @@
         <v>5.160000000000004</v>
       </c>
       <c r="B210" t="n">
-        <v>0.04651162790696634</v>
+        <v>0.0465116279069545</v>
       </c>
     </row>
     <row r="211">
@@ -2055,7 +2055,7 @@
         <v>5.180000000000003</v>
       </c>
       <c r="B211" t="n">
-        <v>0.04633204633195505</v>
+        <v>0.04633204633202429</v>
       </c>
     </row>
     <row r="212">
@@ -2063,7 +2063,7 @@
         <v>5.200000000000004</v>
       </c>
       <c r="B212" t="n">
-        <v>0.0461538461538096</v>
+        <v>0.04615384615382138</v>
       </c>
     </row>
     <row r="213">
@@ -2071,7 +2071,7 @@
         <v>5.220000000000004</v>
       </c>
       <c r="B213" t="n">
-        <v>0.04597701149424383</v>
+        <v>0.0459770114942256</v>
       </c>
     </row>
     <row r="214">
@@ -2079,7 +2079,7 @@
         <v>5.240000000000004</v>
       </c>
       <c r="B214" t="n">
-        <v>0.0458015267175363</v>
+        <v>0.04580152671753738</v>
       </c>
     </row>
     <row r="215">
@@ -2087,7 +2087,7 @@
         <v>5.260000000000003</v>
       </c>
       <c r="B215" t="n">
-        <v>0.04562737642594584</v>
+        <v>0.04562737642583096</v>
       </c>
     </row>
     <row r="216">
@@ -2095,7 +2095,7 @@
         <v>5.280000000000004</v>
       </c>
       <c r="B216" t="n">
-        <v>0.04545454545451957</v>
+        <v>0.04545454545452834</v>
       </c>
     </row>
     <row r="217">
@@ -2103,7 +2103,7 @@
         <v>5.300000000000004</v>
       </c>
       <c r="B217" t="n">
-        <v>0.04528301886795279</v>
+        <v>0.04528301886790143</v>
       </c>
     </row>
     <row r="218">
@@ -2111,7 +2111,7 @@
         <v>5.320000000000004</v>
       </c>
       <c r="B218" t="n">
-        <v>0.04511278195460621</v>
+        <v>0.04511278195487048</v>
       </c>
     </row>
     <row r="219">
@@ -2119,7 +2119,7 @@
         <v>5.340000000000003</v>
       </c>
       <c r="B219" t="n">
-        <v>0.04494382022472806</v>
+        <v>0.04494382022469853</v>
       </c>
     </row>
     <row r="220">
@@ -2127,7 +2127,7 @@
         <v>5.360000000000004</v>
       </c>
       <c r="B220" t="n">
-        <v>0.04477611940280941</v>
+        <v>0.04477611940296265</v>
       </c>
     </row>
     <row r="221">
@@ -2135,7 +2135,7 @@
         <v>5.380000000000004</v>
       </c>
       <c r="B221" t="n">
-        <v>0.04460966542746247</v>
+        <v>0.04460966542748489</v>
       </c>
     </row>
     <row r="222">
@@ -2143,7 +2143,7 @@
         <v>5.400000000000004</v>
       </c>
       <c r="B222" t="n">
-        <v>0.04444444444450258</v>
+        <v>0.0444444444444179</v>
       </c>
     </row>
     <row r="223">
@@ -2151,7 +2151,7 @@
         <v>5.420000000000003</v>
       </c>
       <c r="B223" t="n">
-        <v>0.04428044280435557</v>
+        <v>0.0442804428043975</v>
       </c>
     </row>
     <row r="224">
@@ -2159,7 +2159,7 @@
         <v>5.440000000000004</v>
       </c>
       <c r="B224" t="n">
-        <v>0.04411764705878941</v>
+        <v>0.04411764705879895</v>
       </c>
     </row>
     <row r="225">
@@ -2167,7 +2167,7 @@
         <v>5.460000000000004</v>
       </c>
       <c r="B225" t="n">
-        <v>0.04395604395597182</v>
+        <v>0.0439560439560405</v>
       </c>
     </row>
     <row r="226">
@@ -2175,7 +2175,7 @@
         <v>5.480000000000004</v>
       </c>
       <c r="B226" t="n">
-        <v>0.04379562043773861</v>
+        <v>0.04379562043794698</v>
       </c>
     </row>
     <row r="227">
@@ -2183,7 +2183,7 @@
         <v>5.500000000000004</v>
       </c>
       <c r="B227" t="n">
-        <v>0.0436363636361477</v>
+        <v>0.04363636363634691</v>
       </c>
     </row>
     <row r="228">
@@ -2191,7 +2191,7 @@
         <v>5.520000000000004</v>
       </c>
       <c r="B228" t="n">
-        <v>0.04347826086941756</v>
+        <v>0.04347826086954307</v>
       </c>
     </row>
     <row r="229">
@@ -2199,7 +2199,7 @@
         <v>5.540000000000004</v>
       </c>
       <c r="B229" t="n">
-        <v>0.043321299638774</v>
+        <v>0.04332129963896191</v>
       </c>
     </row>
     <row r="230">
@@ -2207,7 +2207,7 @@
         <v>5.560000000000004</v>
       </c>
       <c r="B230" t="n">
-        <v>0.04316546762565941</v>
+        <v>0.04316546762590332</v>
       </c>
     </row>
     <row r="231">
@@ -2215,7 +2215,7 @@
         <v>5.580000000000004</v>
       </c>
       <c r="B231" t="n">
-        <v>0.04301075268818457</v>
+        <v>0.04301075268817973</v>
       </c>
     </row>
     <row r="232">
@@ -2223,7 +2223,7 @@
         <v>5.600000000000004</v>
       </c>
       <c r="B232" t="n">
-        <v>0.04285714285708468</v>
+        <v>0.04285714285714926</v>
       </c>
     </row>
     <row r="233">
@@ -2231,7 +2231,7 @@
         <v>5.620000000000005</v>
       </c>
       <c r="B233" t="n">
-        <v>0.04270462633420211</v>
+        <v>0.04270462633452016</v>
       </c>
     </row>
     <row r="234">
@@ -2239,7 +2239,7 @@
         <v>5.640000000000004</v>
       </c>
       <c r="B234" t="n">
-        <v>0.04255319148917364</v>
+        <v>0.04255319148936253</v>
       </c>
     </row>
     <row r="235">
@@ -2247,7 +2247,7 @@
         <v>5.660000000000004</v>
       </c>
       <c r="B235" t="n">
-        <v>0.04240282685507333</v>
+        <v>0.04240282685514119</v>
       </c>
     </row>
     <row r="236">
@@ -2255,7 +2255,7 @@
         <v>5.680000000000004</v>
       </c>
       <c r="B236" t="n">
-        <v>0.04225352112670907</v>
+        <v>0.04225352112678397</v>
       </c>
     </row>
     <row r="237">
@@ -2263,7 +2263,7 @@
         <v>5.700000000000005</v>
       </c>
       <c r="B237" t="n">
-        <v>0.04210526315786573</v>
+        <v>0.04210526315793929</v>
       </c>
     </row>
     <row r="238">
@@ -2271,7 +2271,7 @@
         <v>5.720000000000004</v>
       </c>
       <c r="B238" t="n">
-        <v>0.04195804195795693</v>
+        <v>0.0419580419580255</v>
       </c>
     </row>
     <row r="239">
@@ -2279,7 +2279,7 @@
         <v>5.740000000000004</v>
       </c>
       <c r="B239" t="n">
-        <v>0.04181184668976971</v>
+        <v>0.04181184668988434</v>
       </c>
     </row>
     <row r="240">
@@ -2287,7 +2287,7 @@
         <v>5.760000000000004</v>
       </c>
       <c r="B240" t="n">
-        <v>0.04166666666670856</v>
+        <v>0.04166666666664324</v>
       </c>
     </row>
     <row r="241">
@@ -2295,7 +2295,7 @@
         <v>5.780000000000005</v>
       </c>
       <c r="B241" t="n">
-        <v>0.0415224913496224</v>
+        <v>0.04152249134945477</v>
       </c>
     </row>
     <row r="242">
@@ -2303,7 +2303,7 @@
         <v>5.800000000000004</v>
       </c>
       <c r="B242" t="n">
-        <v>0.0413793103446394</v>
+        <v>0.04137931034479703</v>
       </c>
     </row>
     <row r="243">
@@ -2311,7 +2311,7 @@
         <v>5.820000000000004</v>
       </c>
       <c r="B243" t="n">
-        <v>0.0412371134019055</v>
+        <v>0.0412371134020277</v>
       </c>
     </row>
     <row r="244">
@@ -2319,7 +2319,7 @@
         <v>5.840000000000004</v>
       </c>
       <c r="B244" t="n">
-        <v>0.04109589041094873</v>
+        <v>0.04109589041092804</v>
       </c>
     </row>
     <row r="245">
@@ -2327,7 +2327,7 @@
         <v>5.860000000000005</v>
       </c>
       <c r="B245" t="n">
-        <v>0.04095563139923604</v>
+        <v>0.0409556313993668</v>
       </c>
     </row>
     <row r="246">
@@ -2335,7 +2335,7 @@
         <v>5.880000000000004</v>
       </c>
       <c r="B246" t="n">
-        <v>0.04081632653044708</v>
+        <v>0.04081632653063883</v>
       </c>
     </row>
     <row r="247">
@@ -2343,7 +2343,7 @@
         <v>5.900000000000004</v>
       </c>
       <c r="B247" t="n">
-        <v>0.0406779661015518</v>
+        <v>0.04067796610168675</v>
       </c>
     </row>
     <row r="248">
@@ -2351,7 +2351,7 @@
         <v>5.920000000000004</v>
       </c>
       <c r="B248" t="n">
-        <v>0.04054054054056822</v>
+        <v>0.04054054054053904</v>
       </c>
     </row>
     <row r="249">
@@ -2359,7 +2359,7 @@
         <v>5.940000000000005</v>
       </c>
       <c r="B249" t="n">
-        <v>0.04040404040391463</v>
+        <v>0.04040404040433097</v>
       </c>
     </row>
     <row r="250">
@@ -2367,7 +2367,7 @@
         <v>5.960000000000004</v>
       </c>
       <c r="B250" t="n">
-        <v>0.04026845637557522</v>
+        <v>0.0402684563759593</v>
       </c>
     </row>
     <row r="251">
@@ -2375,7 +2375,7 @@
         <v>5.980000000000004</v>
       </c>
       <c r="B251" t="n">
-        <v>0.04013377926419039</v>
+        <v>0.04013377926436023</v>
       </c>
     </row>
     <row r="252">
@@ -2383,7 +2383,7 @@
         <v>6.000000000000004</v>
       </c>
       <c r="B252" t="n">
-        <v>0.03999999999990923</v>
+        <v>0.04000000000013505</v>
       </c>
     </row>
     <row r="253">
@@ -2391,7 +2391,7 @@
         <v>6.020000000000005</v>
       </c>
       <c r="B253" t="n">
-        <v>0.03986710963443245</v>
+        <v>0.03986710963469529</v>
       </c>
     </row>
     <row r="254">
@@ -2399,7 +2399,7 @@
         <v>6.040000000000004</v>
       </c>
       <c r="B254" t="n">
-        <v>0.03973509933748612</v>
+        <v>0.03973509933788794</v>
       </c>
     </row>
     <row r="255">
@@ -2407,7 +2407,7 @@
         <v>6.060000000000004</v>
       </c>
       <c r="B255" t="n">
-        <v>0.03960396039596135</v>
+        <v>0.03960396039618336</v>
       </c>
     </row>
     <row r="256">
@@ -2415,7 +2415,7 @@
         <v>6.080000000000005</v>
       </c>
       <c r="B256" t="n">
-        <v>0.03947368421059388</v>
+        <v>0.03947368421067068</v>
       </c>
     </row>
     <row r="257">
@@ -2423,7 +2423,7 @@
         <v>6.100000000000005</v>
       </c>
       <c r="B257" t="n">
-        <v>0.03934426229494907</v>
+        <v>0.03934426229521477</v>
       </c>
     </row>
     <row r="258">
@@ -2431,7 +2431,7 @@
         <v>6.120000000000005</v>
       </c>
       <c r="B258" t="n">
-        <v>0.03921568627452573</v>
+        <v>0.03921568627463828</v>
       </c>
     </row>
     <row r="259">
@@ -2439,7 +2439,7 @@
         <v>6.140000000000004</v>
       </c>
       <c r="B259" t="n">
-        <v>0.03908794788260388</v>
+        <v>0.03908794788286396</v>
       </c>
     </row>
     <row r="260">
@@ -2447,7 +2447,7 @@
         <v>6.160000000000005</v>
       </c>
       <c r="B260" t="n">
-        <v>0.03896103896096233</v>
+        <v>0.03896103896101266</v>
       </c>
     </row>
     <row r="261">
@@ -2455,7 +2455,7 @@
         <v>6.180000000000005</v>
       </c>
       <c r="B261" t="n">
-        <v>0.03883495145625789</v>
+        <v>0.03883495145626441</v>
       </c>
     </row>
     <row r="262">
@@ -2463,7 +2463,7 @@
         <v>6.200000000000005</v>
       </c>
       <c r="B262" t="n">
-        <v>0.03870967741926058</v>
+        <v>0.03870967741933081</v>
       </c>
     </row>
     <row r="263">
@@ -2471,7 +2471,7 @@
         <v>6.220000000000004</v>
       </c>
       <c r="B263" t="n">
-        <v>0.03858520900317316</v>
+        <v>0.0385852090031851</v>
       </c>
     </row>
     <row r="264">
@@ -2479,7 +2479,7 @@
         <v>6.240000000000005</v>
       </c>
       <c r="B264" t="n">
-        <v>0.03846153846133044</v>
+        <v>0.03846153846150507</v>
       </c>
     </row>
     <row r="265">
@@ -2487,7 +2487,7 @@
         <v>6.260000000000005</v>
       </c>
       <c r="B265" t="n">
-        <v>0.03833865814693529</v>
+        <v>0.03833865814694806</v>
       </c>
     </row>
     <row r="266">
@@ -2495,7 +2495,7 @@
         <v>6.280000000000005</v>
       </c>
       <c r="B266" t="n">
-        <v>0.03821656050941263</v>
+        <v>0.03821656050954127</v>
       </c>
     </row>
     <row r="267">
@@ -2503,7 +2503,7 @@
         <v>6.300000000000004</v>
       </c>
       <c r="B267" t="n">
-        <v>0.038095238095372</v>
+        <v>0.03809523809523121</v>
       </c>
     </row>
     <row r="268">
@@ -2511,7 +2511,7 @@
         <v>6.320000000000005</v>
       </c>
       <c r="B268" t="n">
-        <v>0.03797468354416517</v>
+        <v>0.03797468354429009</v>
       </c>
     </row>
     <row r="269">
@@ -2519,7 +2519,7 @@
         <v>6.340000000000005</v>
       </c>
       <c r="B269" t="n">
-        <v>0.03785488958973165</v>
+        <v>0.03785488958986145</v>
       </c>
     </row>
     <row r="270">
@@ -2527,7 +2527,7 @@
         <v>6.360000000000005</v>
       </c>
       <c r="B270" t="n">
-        <v>0.03773584905636528</v>
+        <v>0.03773584905661401</v>
       </c>
     </row>
     <row r="271">
@@ -2535,7 +2535,7 @@
         <v>6.380000000000004</v>
       </c>
       <c r="B271" t="n">
-        <v>0.03761755485880387</v>
+        <v>0.03761755485886045</v>
       </c>
     </row>
     <row r="272">
@@ -2543,7 +2543,7 @@
         <v>6.400000000000005</v>
       </c>
       <c r="B272" t="n">
-        <v>0.03749999999984992</v>
+        <v>0.03750000000000299</v>
       </c>
     </row>
     <row r="273">
@@ -2551,7 +2551,7 @@
         <v>6.420000000000005</v>
       </c>
       <c r="B273" t="n">
-        <v>0.03738317756986333</v>
+        <v>0.03738317757009704</v>
       </c>
     </row>
     <row r="274">
@@ -2559,7 +2559,7 @@
         <v>6.440000000000005</v>
       </c>
       <c r="B274" t="n">
-        <v>0.03726708074530696</v>
+        <v>0.03726708074519039</v>
       </c>
     </row>
     <row r="275">
@@ -2567,7 +2567,7 @@
         <v>6.460000000000004</v>
       </c>
       <c r="B275" t="n">
-        <v>0.0371517027863623</v>
+        <v>0.03715170278623348</v>
       </c>
     </row>
     <row r="276">
@@ -2575,7 +2575,7 @@
         <v>6.480000000000005</v>
       </c>
       <c r="B276" t="n">
-        <v>0.03703703703717085</v>
+        <v>0.03703703703708432</v>
       </c>
     </row>
     <row r="277">
@@ -2583,7 +2583,7 @@
         <v>6.500000000000005</v>
       </c>
       <c r="B277" t="n">
-        <v>0.03692307692295223</v>
+        <v>0.03692307692333424</v>
       </c>
     </row>
     <row r="278">
@@ -2591,7 +2591,7 @@
         <v>6.520000000000005</v>
       </c>
       <c r="B278" t="n">
-        <v>0.03680981595091715</v>
+        <v>0.03680981595092361</v>
       </c>
     </row>
     <row r="279">
@@ -2599,7 +2599,7 @@
         <v>6.540000000000004</v>
       </c>
       <c r="B279" t="n">
-        <v>0.03669724770635194</v>
+        <v>0.0366972477064241</v>
       </c>
     </row>
     <row r="280">
@@ -2607,7 +2607,7 @@
         <v>6.560000000000005</v>
       </c>
       <c r="B280" t="n">
-        <v>0.03658536585360285</v>
+        <v>0.03658536585344696</v>
       </c>
     </row>
     <row r="281">
@@ -2615,7 +2615,7 @@
         <v>6.580000000000005</v>
       </c>
       <c r="B281" t="n">
-        <v>0.03647416413378669</v>
+        <v>0.03647416413371194</v>
       </c>
     </row>
     <row r="282">
@@ -2623,7 +2623,7 @@
         <v>6.600000000000005</v>
       </c>
       <c r="B282" t="n">
-        <v>0.03636363636362402</v>
+        <v>0.03636363636361169</v>
       </c>
     </row>
     <row r="283">
@@ -2631,7 +2631,7 @@
         <v>6.620000000000005</v>
       </c>
       <c r="B283" t="n">
-        <v>0.0362537764350515</v>
+        <v>0.03625377643502176</v>
       </c>
     </row>
     <row r="284">
@@ -2639,7 +2639,7 @@
         <v>6.640000000000005</v>
       </c>
       <c r="B284" t="n">
-        <v>0.03614457831297591</v>
+        <v>0.03614457831322969</v>
       </c>
     </row>
     <row r="285">
@@ -2647,7 +2647,7 @@
         <v>6.660000000000005</v>
       </c>
       <c r="B285" t="n">
-        <v>0.03603603603602328</v>
+        <v>0.03603603603602971</v>
       </c>
     </row>
     <row r="286">
@@ -2655,7 +2655,7 @@
         <v>6.680000000000005</v>
       </c>
       <c r="B286" t="n">
-        <v>0.03592814371250699</v>
+        <v>0.03592814371256838</v>
       </c>
     </row>
     <row r="287">
@@ -2663,7 +2663,7 @@
         <v>6.700000000000005</v>
       </c>
       <c r="B287" t="n">
-        <v>0.03582089552204495</v>
+        <v>0.03582089552238177</v>
       </c>
     </row>
     <row r="288">
@@ -2671,7 +2671,7 @@
         <v>6.720000000000005</v>
       </c>
       <c r="B288" t="n">
-        <v>0.03571428571416962</v>
+        <v>0.03571428571427886</v>
       </c>
     </row>
     <row r="289">
@@ -2679,7 +2679,7 @@
         <v>6.740000000000006</v>
       </c>
       <c r="B289" t="n">
-        <v>0.03560830860519285</v>
+        <v>0.0356083086053348</v>
       </c>
     </row>
     <row r="290">
@@ -2687,7 +2687,7 @@
         <v>6.760000000000005</v>
       </c>
       <c r="B290" t="n">
-        <v>0.03550295857990378</v>
+        <v>0.03550295857987455</v>
       </c>
     </row>
     <row r="291">
@@ -2695,7 +2695,7 @@
         <v>6.780000000000005</v>
       </c>
       <c r="B291" t="n">
-        <v>0.03539823008833962</v>
+        <v>0.03539823008848916</v>
       </c>
     </row>
     <row r="292">
@@ -2703,7 +2703,7 @@
         <v>6.800000000000005</v>
       </c>
       <c r="B292" t="n">
-        <v>0.03529411764689847</v>
+        <v>0.03529411764705349</v>
       </c>
     </row>
     <row r="293">
@@ -2711,7 +2711,7 @@
         <v>6.820000000000006</v>
       </c>
       <c r="B293" t="n">
-        <v>0.03519061583569456</v>
+        <v>0.03519061583577113</v>
       </c>
     </row>
     <row r="294">
@@ -2719,7 +2719,7 @@
         <v>6.840000000000005</v>
       </c>
       <c r="B294" t="n">
-        <v>0.03508771929834795</v>
+        <v>0.03508771929824014</v>
       </c>
     </row>
     <row r="295">
@@ -2727,7 +2727,7 @@
         <v>6.860000000000005</v>
       </c>
       <c r="B295" t="n">
-        <v>0.03498542274043578</v>
+        <v>0.03498542274098039</v>
       </c>
     </row>
     <row r="296">
@@ -2735,7 +2735,7 @@
         <v>6.880000000000005</v>
       </c>
       <c r="B296" t="n">
-        <v>0.03488372093019747</v>
+        <v>0.03488372093030542</v>
       </c>
     </row>
     <row r="297">
@@ -2743,7 +2743,7 @@
         <v>6.900000000000006</v>
       </c>
       <c r="B297" t="n">
-        <v>0.03478260869561241</v>
+        <v>0.03478260869611277</v>
       </c>
     </row>
     <row r="298">
@@ -2751,7 +2751,7 @@
         <v>6.920000000000005</v>
       </c>
       <c r="B298" t="n">
-        <v>0.03468208092472566</v>
+        <v>0.03468208092407363</v>
       </c>
     </row>
     <row r="299">
@@ -2759,7 +2759,7 @@
         <v>6.940000000000005</v>
       </c>
       <c r="B299" t="n">
-        <v>0.03458213256470506</v>
+        <v>0.03458213256468921</v>
       </c>
     </row>
     <row r="300">
@@ -2767,7 +2767,7 @@
         <v>6.960000000000005</v>
       </c>
       <c r="B300" t="n">
-        <v>0.03448275862060435</v>
+        <v>0.03448275862053653</v>
       </c>
     </row>
     <row r="301">
@@ -2775,7 +2775,7 @@
         <v>6.980000000000006</v>
       </c>
       <c r="B301" t="n">
-        <v>0.03438395415473251</v>
+        <v>0.03438395415457789</v>
       </c>
     </row>
     <row r="302">
@@ -2783,7 +2783,7 @@
         <v>7.000000000000005</v>
       </c>
       <c r="B302" t="n">
-        <v>0.034285714286016</v>
+        <v>0.03428571428568404</v>
       </c>
     </row>
     <row r="303">
@@ -2791,7 +2791,7 @@
         <v>7.020000000000005</v>
       </c>
       <c r="B303" t="n">
-        <v>0.03418803418800952</v>
+        <v>0.03418803418800077</v>
       </c>
     </row>
     <row r="304">
@@ -2799,7 +2799,7 @@
         <v>7.040000000000005</v>
       </c>
       <c r="B304" t="n">
-        <v>0.03409090909093419</v>
+        <v>0.03409090909090738</v>
       </c>
     </row>
     <row r="305">
@@ -2807,7 +2807,7 @@
         <v>7.060000000000006</v>
       </c>
       <c r="B305" t="n">
-        <v>0.03399433427774733</v>
+        <v>0.03399433427760739</v>
       </c>
     </row>
     <row r="306">
@@ -2815,7 +2815,7 @@
         <v>7.080000000000005</v>
       </c>
       <c r="B306" t="n">
-        <v>0.03389830508475027</v>
+        <v>0.03389830508472352</v>
       </c>
     </row>
     <row r="307">
@@ -2823,7 +2823,7 @@
         <v>7.100000000000005</v>
       </c>
       <c r="B307" t="n">
-        <v>0.03380281690144311</v>
+        <v>0.0338028169013579</v>
       </c>
     </row>
     <row r="308">
@@ -2831,7 +2831,7 @@
         <v>7.120000000000005</v>
       </c>
       <c r="B308" t="n">
-        <v>0.03370786516861239</v>
+        <v>0.03370786516850244</v>
       </c>
     </row>
     <row r="309">
@@ -2839,7 +2839,7 @@
         <v>7.140000000000006</v>
       </c>
       <c r="B309" t="n">
-        <v>0.0336134453782785</v>
+        <v>0.03361344537811361</v>
       </c>
     </row>
     <row r="310">
@@ -2847,7 +2847,7 @@
         <v>7.160000000000005</v>
       </c>
       <c r="B310" t="n">
-        <v>0.0335195530725758</v>
+        <v>0.03351955307261056</v>
       </c>
     </row>
     <row r="311">
@@ -2855,7 +2855,7 @@
         <v>7.180000000000005</v>
       </c>
       <c r="B311" t="n">
-        <v>0.03342618384366779</v>
+        <v>0.03342618384399668</v>
       </c>
     </row>
     <row r="312">
@@ -2863,7 +2863,7 @@
         <v>7.200000000000006</v>
       </c>
       <c r="B312" t="n">
-        <v>0.03333333333339628</v>
+        <v>0.03333333333331917</v>
       </c>
     </row>
     <row r="313">
@@ -2871,7 +2871,7 @@
         <v>7.220000000000006</v>
       </c>
       <c r="B313" t="n">
-        <v>0.03324099722997412</v>
+        <v>0.03324099722989841</v>
       </c>
     </row>
     <row r="314">
@@ -2879,7 +2879,7 @@
         <v>7.240000000000006</v>
       </c>
       <c r="B314" t="n">
-        <v>0.03314917127079361</v>
+        <v>0.03314917127072875</v>
       </c>
     </row>
     <row r="315">
@@ -2887,7 +2887,7 @@
         <v>7.260000000000005</v>
       </c>
       <c r="B315" t="n">
-        <v>0.0330578512393821</v>
+        <v>0.03305785123968052</v>
       </c>
     </row>
     <row r="316">
@@ -2895,7 +2895,7 @@
         <v>7.280000000000006</v>
       </c>
       <c r="B316" t="n">
-        <v>0.03296703296699008</v>
+        <v>0.03296703296704166</v>
       </c>
     </row>
     <row r="317">
@@ -2903,7 +2903,7 @@
         <v>7.300000000000006</v>
       </c>
       <c r="B317" t="n">
-        <v>0.03287671232869666</v>
+        <v>0.03287671232875933</v>
       </c>
     </row>
     <row r="318">
@@ -2911,7 +2911,7 @@
         <v>7.320000000000006</v>
       </c>
       <c r="B318" t="n">
-        <v>0.03278688524587514</v>
+        <v>0.03278688524589307</v>
       </c>
     </row>
     <row r="319">
@@ -2919,7 +2919,7 @@
         <v>7.340000000000005</v>
       </c>
       <c r="B319" t="n">
-        <v>0.03269754768382695</v>
+        <v>0.03269754768390843</v>
       </c>
     </row>
     <row r="320">
@@ -2927,7 +2927,7 @@
         <v>7.360000000000006</v>
       </c>
       <c r="B320" t="n">
-        <v>0.03260869565205735</v>
+        <v>0.03260869565216059</v>
       </c>
     </row>
     <row r="321">
@@ -2935,7 +2935,7 @@
         <v>7.380000000000006</v>
       </c>
       <c r="B321" t="n">
-        <v>0.03252032520334253</v>
+        <v>0.03252032520323637</v>
       </c>
     </row>
     <row r="322">
@@ -2943,7 +2943,7 @@
         <v>7.400000000000006</v>
       </c>
       <c r="B322" t="n">
-        <v>0.03243243243259367</v>
+        <v>0.03243243243242185</v>
       </c>
     </row>
     <row r="323">
@@ -2951,7 +2951,7 @@
         <v>7.420000000000005</v>
       </c>
       <c r="B323" t="n">
-        <v>0.03234501347724337</v>
+        <v>0.03234501347708747</v>
       </c>
     </row>
     <row r="324">
@@ -2959,7 +2959,7 @@
         <v>7.440000000000006</v>
       </c>
       <c r="B324" t="n">
-        <v>0.03225806451609792</v>
+        <v>0.03225806451611968</v>
       </c>
     </row>
     <row r="325">
@@ -2967,7 +2967,7 @@
         <v>7.460000000000006</v>
       </c>
       <c r="B325" t="n">
-        <v>0.03217158176933882</v>
+        <v>0.03217158176942595</v>
       </c>
     </row>
     <row r="326">
@@ -2975,7 +2975,7 @@
         <v>7.480000000000006</v>
       </c>
       <c r="B326" t="n">
-        <v>0.03208556149728933</v>
+        <v>0.03208556149731271</v>
       </c>
     </row>
     <row r="327">
@@ -2983,7 +2983,7 @@
         <v>7.500000000000005</v>
       </c>
       <c r="B327" t="n">
-        <v>0.03199999999998356</v>
+        <v>0.03200000000000423</v>
       </c>
     </row>
     <row r="328">
@@ -2991,7 +2991,7 @@
         <v>7.520000000000006</v>
       </c>
       <c r="B328" t="n">
-        <v>0.03191489361688648</v>
+        <v>0.03191489361700849</v>
       </c>
     </row>
     <row r="329">
@@ -2999,7 +2999,7 @@
         <v>7.540000000000006</v>
       </c>
       <c r="B329" t="n">
-        <v>0.03183023872661477</v>
+        <v>0.03183023872645009</v>
       </c>
     </row>
     <row r="330">
@@ -3007,7 +3007,7 @@
         <v>7.560000000000006</v>
       </c>
       <c r="B330" t="n">
-        <v>0.03174603174591969</v>
+        <v>0.03174603174566832</v>
       </c>
     </row>
     <row r="331">
@@ -3015,7 +3015,7 @@
         <v>7.580000000000005</v>
       </c>
       <c r="B331" t="n">
-        <v>0.03166226912925002</v>
+        <v>0.0316622691292579</v>
       </c>
     </row>
     <row r="332">
@@ -3023,7 +3023,7 @@
         <v>7.600000000000006</v>
       </c>
       <c r="B332" t="n">
-        <v>0.03157894736854193</v>
+        <v>0.03157894736842082</v>
       </c>
     </row>
     <row r="333">
@@ -3031,7 +3031,7 @@
         <v>7.620000000000006</v>
       </c>
       <c r="B333" t="n">
-        <v>0.03149606299199981</v>
+        <v>0.03149606299207748</v>
       </c>
     </row>
     <row r="334">
@@ -3039,7 +3039,7 @@
         <v>7.640000000000006</v>
       </c>
       <c r="B334" t="n">
-        <v>0.0314136125653448</v>
+        <v>0.0314136125653677</v>
       </c>
     </row>
     <row r="335">
@@ -3047,7 +3047,7 @@
         <v>7.660000000000005</v>
       </c>
       <c r="B335" t="n">
-        <v>0.03133159268924052</v>
+        <v>0.03133159268927203</v>
       </c>
     </row>
     <row r="336">
@@ -3055,7 +3055,7 @@
         <v>7.680000000000006</v>
       </c>
       <c r="B336" t="n">
-        <v>0.03125000000005602</v>
+        <v>0.03124999999997426</v>
       </c>
     </row>
     <row r="337">
@@ -3063,7 +3063,7 @@
         <v>7.700000000000006</v>
       </c>
       <c r="B337" t="n">
-        <v>0.03116883116879559</v>
+        <v>0.03116883116868391</v>
       </c>
     </row>
     <row r="338">
@@ -3071,7 +3071,7 @@
         <v>7.720000000000006</v>
       </c>
       <c r="B338" t="n">
-        <v>0.03108808290160663</v>
+        <v>0.03108808290140808</v>
       </c>
     </row>
     <row r="339">
@@ -3079,7 +3079,7 @@
         <v>7.740000000000006</v>
       </c>
       <c r="B339" t="n">
-        <v>0.03100775193805771</v>
+        <v>0.03100775193796383</v>
       </c>
     </row>
     <row r="340">
@@ -3087,7 +3087,7 @@
         <v>7.760000000000006</v>
       </c>
       <c r="B340" t="n">
-        <v>0.03092783505131014</v>
+        <v>0.03092783505151609</v>
       </c>
     </row>
     <row r="341">
@@ -3095,7 +3095,7 @@
         <v>7.780000000000006</v>
       </c>
       <c r="B341" t="n">
-        <v>0.03084832904869813</v>
+        <v>0.03084832904881124</v>
       </c>
     </row>
     <row r="342">
@@ -3103,7 +3103,7 @@
         <v>7.800000000000006</v>
       </c>
       <c r="B342" t="n">
-        <v>0.03076923076922617</v>
+        <v>0.03076923076921918</v>
       </c>
     </row>
     <row r="343">
@@ -3111,7 +3111,7 @@
         <v>7.820000000000006</v>
       </c>
       <c r="B343" t="n">
-        <v>0.03069053708442086</v>
+        <v>0.03069053708438711</v>
       </c>
     </row>
     <row r="344">
@@ -3119,7 +3119,7 @@
         <v>7.840000000000006</v>
       </c>
       <c r="B344" t="n">
-        <v>0.03061224489796638</v>
+        <v>0.03061224489794813</v>
       </c>
     </row>
     <row r="345">
@@ -3127,7 +3127,7 @@
         <v>7.860000000000007</v>
       </c>
       <c r="B345" t="n">
-        <v>0.03053435114497606</v>
+        <v>0.03053435114501823</v>
       </c>
     </row>
     <row r="346">
@@ -3135,7 +3135,7 @@
         <v>7.880000000000006</v>
       </c>
       <c r="B346" t="n">
-        <v>0.03045685279197938</v>
+        <v>0.03045685279197263</v>
       </c>
     </row>
     <row r="347">
@@ -3143,7 +3143,7 @@
         <v>7.900000000000006</v>
       </c>
       <c r="B347" t="n">
-        <v>0.03037974683537965</v>
+        <v>0.03037974683539888</v>
       </c>
     </row>
     <row r="348">
@@ -3151,7 +3151,7 @@
         <v>7.920000000000006</v>
       </c>
       <c r="B348" t="n">
-        <v>0.0303030303028473</v>
+        <v>0.03030303030301138</v>
       </c>
     </row>
     <row r="349">
@@ -3159,7 +3159,7 @@
         <v>7.940000000000007</v>
       </c>
       <c r="B349" t="n">
-        <v>0.03022670025176689</v>
+        <v>0.03022670025185887</v>
       </c>
     </row>
     <row r="350">
@@ -3167,7 +3167,7 @@
         <v>7.960000000000006</v>
       </c>
       <c r="B350" t="n">
-        <v>0.0301507537687762</v>
+        <v>0.03015075376881178</v>
       </c>
     </row>
     <row r="351">
@@ -3175,7 +3175,15 @@
         <v>7.980000000000006</v>
       </c>
       <c r="B351" t="n">
-        <v>0.03007518796985947</v>
+        <v>0.03007518796994717</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>8.000000000000007</v>
+      </c>
+      <c r="B352" t="n">
+        <v>0.03000000000002982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>